<commit_message>
feat: :test_tube: Testing with more study guides on spanish
</commit_message>
<xml_diff>
--- a/flashcards/flashcards.xlsx
+++ b/flashcards/flashcards.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,123 +413,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Question</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Answer</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Q1: What is the definition of programming?</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>A1: The process of writing instructions for a computer to perform specific tasks.</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Q2: What is an algorithm?</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>A2: An step-by-step procedure for solving a problem.</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Q3: What is a programming language?</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>A3: A formal language used to communicate instructions to a machine.</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Q4: What is syntax in the context of programming?</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>A4: The rules defining the structure of a programming language.</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Q5: What does debugging refer to in programming?</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>A5: The process of finding and fixing errors in code.</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Q6: What is a variable in programming?</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>A6: A named storage location for data.</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Q7: What are some common data types in programming?</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>A7: `int`, `float`, `string` are examples of common data types in programming.</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Q8: Provide an example of variable and its assignment in Python.</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>A8: `name = "Alice"` and `age = 25` are examples of variable and their assignments in Python.</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: :fire: More tests and modified README
</commit_message>
<xml_diff>
--- a/flashcards/flashcards.xlsx
+++ b/flashcards/flashcards.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,123 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Question</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Answer</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Q1: ¿Qué es una red en telecomunicaciones?</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>A1: Una red es un conjunto de dispositivos interconectados que permiten la comunicación entre sí.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Q2: ¿Cuál es la función de un router en una red?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>A2: El router se encarga de dirigir el tráfico de datos entre diferentes redes o segmentos de red.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Q3: ¿Qué son las capas del modelo OSI y cuál es su número?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>A3: Las capas del modelo OSI son siete y van desde la física hasta la aplicación, siendo cada una responsable de una parte específica de la comunicación.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Q4: ¿Cuál es el protocolo de transmisión de datos en la capa de red del modelo OSI?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>A4: El protocolo de transmisión de datos en la capa de red es IP (Internet Protocol).</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Q5: ¿Qué son los nodos en una red y cuál es su función?</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>A5: Los nodos son dispositivos o puntos de interconexión en una red. Sus funciones pueden variar dependiendo del tipo de nodo, pero generalmente se encargan de la recepción, procesamiento y envío de datos.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Q6: ¿Qué es un firewall y cuál es su función?</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>A6: Un firewall es un dispositivo que controla el tráfico de red entrante y saliente. Su función es proteger una red o un sistema contra ataques y ciberamenazas.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Q7: ¿Qué son los paquetes en una red?</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>A7: Los paquetes son pequeños bloques de datos que contienen información que se envían por redes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Q8: ¿Cuál es el propósito del protocolo TCP y cuál es su número?</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>A8: El propósito del protocolo TCP es garantizar la integridad, confiabilidad y orden de los datos que se envían por redes. Su número es 6 (capa transporte).</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: :sparkles: Improved dividing into sections function
</commit_message>
<xml_diff>
--- a/flashcards/flashcards.xlsx
+++ b/flashcards/flashcards.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,123 +413,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Question</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Answer</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Q1: ¿Qué es una red en telecomunicaciones?</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>A1: Una red es un conjunto de dispositivos interconectados que permiten la comunicación entre sí.</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Q2: ¿Cuál es la función de un router en una red?</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>A2: El router se encarga de dirigir el tráfico de datos entre diferentes redes o segmentos de red.</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Q3: ¿Qué son las capas del modelo OSI y cuál es su número?</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>A3: Las capas del modelo OSI son siete y van desde la física hasta la aplicación, siendo cada una responsable de una parte específica de la comunicación.</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Q4: ¿Cuál es el protocolo de transmisión de datos en la capa de red del modelo OSI?</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>A4: El protocolo de transmisión de datos en la capa de red es IP (Internet Protocol).</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Q5: ¿Qué son los nodos en una red y cuál es su función?</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>A5: Los nodos son dispositivos o puntos de interconexión en una red. Sus funciones pueden variar dependiendo del tipo de nodo, pero generalmente se encargan de la recepción, procesamiento y envío de datos.</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Q6: ¿Qué es un firewall y cuál es su función?</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>A6: Un firewall es un dispositivo que controla el tráfico de red entrante y saliente. Su función es proteger una red o un sistema contra ataques y ciberamenazas.</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Q7: ¿Qué son los paquetes en una red?</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>A7: Los paquetes son pequeños bloques de datos que contienen información que se envían por redes.</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Q8: ¿Cuál es el propósito del protocolo TCP y cuál es su número?</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>A8: El propósito del protocolo TCP es garantizar la integridad, confiabilidad y orden de los datos que se envían por redes. Su número es 6 (capa transporte).</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>